<commit_message>
correction sur last batch 6413b5ea861b29127673e8c40107a4b995e28c1d
</commit_message>
<xml_diff>
--- a/EvolutionExempleHAS/ig/StructureDefinition-fr-current-medication-composition.xlsx
+++ b/EvolutionExempleHAS/ig/StructureDefinition-fr-current-medication-composition.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-23T14:36:30+00:00</t>
+    <t>2025-10-23T12:45:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3259,7 +3259,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>172</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>197</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" hidden="true">
+    <row r="24">
       <c r="A24" t="s" s="2">
         <v>264</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
         <v>390</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
         <v>432</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
         <v>449</v>
       </c>
@@ -9018,12 +9018,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AO61">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>